<commit_message>
update score for problem 2
</commit_message>
<xml_diff>
--- a/score.xlsx
+++ b/score.xlsx
@@ -1,30 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HocDaiHoc\CS112\Our Exercise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\subjects\uit\cs112\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4F0BDF-5949-4382-BBF7-5BD55E05E78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7640"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Trọng số</t>
   </si>
@@ -99,12 +111,15 @@
   </si>
   <si>
     <t>Tổng</t>
+  </si>
+  <si>
+    <t>no comment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -163,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -175,11 +190,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,11 +473,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -560,6 +574,9 @@
       <c r="D8">
         <v>10</v>
       </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
       <c r="G8">
         <v>10</v>
       </c>
@@ -568,11 +585,9 @@
       </c>
       <c r="K8">
         <f>((C8*0.5+D8*0.5)+(F8*0.5+G8*0.5)+(I8*0.5+J8*0.5))/3</f>
-        <v>5</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="M8" s="7"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -581,6 +596,9 @@
       <c r="D9">
         <v>10</v>
       </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
       <c r="G9">
         <v>10</v>
       </c>
@@ -589,11 +607,9 @@
       </c>
       <c r="K9">
         <f t="shared" ref="K9:K22" si="0">((C9*0.5+D9*0.5)+(F9*0.5+G9*0.5)+(I9*0.5+J9*0.5))/3</f>
-        <v>5</v>
-      </c>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="9"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="O9" s="8"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -602,6 +618,9 @@
       <c r="D10">
         <v>10</v>
       </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
       <c r="G10">
         <v>10</v>
       </c>
@@ -610,7 +629,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
@@ -620,6 +639,9 @@
       <c r="D11">
         <v>10</v>
       </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
       <c r="G11">
         <v>10</v>
       </c>
@@ -628,7 +650,7 @@
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
@@ -638,6 +660,9 @@
       <c r="D12">
         <v>10</v>
       </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
       <c r="G12">
         <v>10</v>
       </c>
@@ -646,7 +671,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
@@ -656,6 +681,12 @@
       <c r="D13">
         <v>10</v>
       </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13">
+        <v>9.75</v>
+      </c>
       <c r="G13">
         <v>10</v>
       </c>
@@ -664,7 +695,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6.625</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
@@ -674,6 +705,9 @@
       <c r="D14">
         <v>10</v>
       </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
       <c r="G14">
         <v>10</v>
       </c>
@@ -682,7 +716,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
@@ -692,6 +726,9 @@
       <c r="D15">
         <v>10</v>
       </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
       <c r="G15">
         <v>10</v>
       </c>
@@ -700,7 +737,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
@@ -710,6 +747,9 @@
       <c r="D16">
         <v>10</v>
       </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
       <c r="G16">
         <v>10</v>
       </c>
@@ -718,7 +758,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
@@ -728,6 +768,9 @@
       <c r="D17">
         <v>10</v>
       </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
       <c r="G17">
         <v>10</v>
       </c>
@@ -736,7 +779,7 @@
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -746,6 +789,12 @@
       <c r="D18">
         <v>10</v>
       </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18">
+        <v>9.75</v>
+      </c>
       <c r="G18">
         <v>10</v>
       </c>
@@ -754,7 +803,7 @@
       </c>
       <c r="K18">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6.625</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -773,6 +822,12 @@
       <c r="D20">
         <v>10</v>
       </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20">
+        <v>9.75</v>
+      </c>
       <c r="G20">
         <v>10</v>
       </c>
@@ -781,7 +836,7 @@
       </c>
       <c r="K20">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6.625</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
@@ -791,6 +846,9 @@
       <c r="D21">
         <v>10</v>
       </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
       <c r="G21">
         <v>10</v>
       </c>
@@ -799,7 +857,7 @@
       </c>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -809,12 +867,18 @@
       <c r="D22">
         <v>10</v>
       </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+      <c r="G22">
+        <v>10</v>
+      </c>
       <c r="J22">
         <v>10</v>
       </c>
       <c r="K22">
         <f t="shared" si="0"/>
-        <v>3.3333333333333335</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>